<commit_message>
auto commit Mon Dec 18 14:53:48 CET 2017
</commit_message>
<xml_diff>
--- a/raw/tables/benefits-drawbacks-pws.xlsx
+++ b/raw/tables/benefits-drawbacks-pws.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Benefits</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Enforceable policies</t>
+  </si>
+  <si>
+    <t>Attacks are simple to carry out</t>
+  </si>
+  <si>
+    <t>Large number of attack vectors</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,10 +442,16 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
auto commit Tue Dec 19 16:42:22 CET 2017
</commit_message>
<xml_diff>
--- a/raw/tables/benefits-drawbacks-pws.xlsx
+++ b/raw/tables/benefits-drawbacks-pws.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="22060" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Benefits</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Fast entry on desktops</t>
   </si>
   <si>
-    <t>Work without identification step</t>
-  </si>
-  <si>
     <t>Revokable by administrator</t>
   </si>
   <si>
@@ -99,13 +96,28 @@
   </si>
   <si>
     <t>Large number of attack vectors</t>
+  </si>
+  <si>
+    <t>Low costs</t>
+  </si>
+  <si>
+    <t>SPs</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Idenpendent of identification</t>
+  </si>
+  <si>
+    <t>Misc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,18 +125,64 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -134,8 +192,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,107 +496,142 @@
     <col min="2" max="2" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C7:C13"/>
+    <mergeCell ref="C14:C15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
auto commit Wed Dec 20 10:22:54 CET 2017
</commit_message>
<xml_diff>
--- a/raw/tables/benefits-drawbacks-pws.xlsx
+++ b/raw/tables/benefits-drawbacks-pws.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="6400" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Benefits</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Adjustable security level</t>
   </si>
   <si>
-    <t>Suboptimal coping strategies</t>
-  </si>
-  <si>
     <t>Memory overload from too many passwords</t>
   </si>
   <si>
@@ -111,13 +108,19 @@
   </si>
   <si>
     <t>Misc</t>
+  </si>
+  <si>
+    <t>Attacks can have severe consequences</t>
+  </si>
+  <si>
+    <t>Coping strategies necessary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,6 +132,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,35 +199,59 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color auto="1"/>
-      </left>
-      <right/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,154 +527,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
-    <col min="2" max="2" width="42.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
-      <c r="B12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="7"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="7"/>
+      <c r="A13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
+      <c r="C14" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="C7:C13"/>
-    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>